<commit_message>
Dodanie nowego przycisku służącego do otwierania pliku exelowskiego z wynikami oraz zaimplementowanie funkcjonalności.
</commit_message>
<xml_diff>
--- a/BMI.xlsx
+++ b/BMI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Data</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>19:04:16</t>
+  </si>
+  <si>
+    <t>08-03-2017</t>
+  </si>
+  <si>
+    <t>15:28:00</t>
+  </si>
+  <si>
+    <t>12-03-2017</t>
+  </si>
+  <si>
+    <t>16:27:59</t>
+  </si>
+  <si>
+    <t>18:47:34</t>
   </si>
 </sst>
 </file>
@@ -455,6 +470,62 @@
         <v>20.875</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>

</xml_diff>